<commit_message>
add state query in transformer decoder
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\detr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5D159-9F22-4826-85DD-27DF67C5F88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C92C869-AA3C-4AD7-8863-54C927A2A949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{62CF9DC0-3108-FB47-B69C-4FAD3B0A17CF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>训练Class和State的loss，Class的loss要明显小于State的loss，State的loss没有明显的收敛</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t>Best for class prediction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>results_pretain_state_finetune_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sta_query</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1159,13 +1171,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1203,15 +1215,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>2196352</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1253,13 +1265,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>2199267</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1303,13 +1315,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>2199267</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>8363414</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1353,15 +1365,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1403,13 +1415,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>-1</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1453,13 +1465,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2422,402 +2434,494 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA5840C-E570-41D3-A054-976C8C11FDEB}">
-  <dimension ref="A2:J33"/>
+  <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="DM37" sqref="DM37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="25.375" customWidth="1"/>
-    <col min="5" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="109.625" customWidth="1"/>
-    <col min="10" max="10" width="46.375" customWidth="1"/>
+    <col min="1" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="5" max="5" width="25.375" customWidth="1"/>
+    <col min="6" max="7" width="24.875" customWidth="1"/>
+    <col min="8" max="8" width="28.875" customWidth="1"/>
+    <col min="9" max="9" width="109.625" customWidth="1"/>
+    <col min="11" max="11" width="46.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>100</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="7" t="b">
+      <c r="F3" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
         <v>100</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="8" t="b">
+      <c r="F4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
         <v>100</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8" t="b">
+      <c r="F5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="8" t="b">
+      <c r="F6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
         <v>50</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="8" t="b">
+      <c r="F7" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
         <v>50</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="8" t="b">
+      <c r="F8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>50</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8" t="s">
+      <c r="B10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <v>100</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="8" t="b">
+      <c r="F10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8" t="s">
+      <c r="B11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>100</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="8" t="b">
+      <c r="F11" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="8" t="s">
+      <c r="B12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
+        <v>100</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="8" t="b">
+      <c r="F12" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
         <v>100</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="8" t="b">
+      <c r="F13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J13" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="14" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9">
         <v>50</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="b">
+      <c r="F14" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="8" customFormat="1" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
-    </row>
-    <row r="17" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
-    </row>
-    <row r="18" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-    </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-    </row>
-    <row r="21" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
-    </row>
-    <row r="22" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
-    </row>
-    <row r="28" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
-    </row>
-    <row r="29" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
-    </row>
-    <row r="30" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
-    </row>
-    <row r="32" spans="1:2" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
-    </row>
-    <row r="33" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>